<commit_message>
Edicion Analisis y Diseño
Actualizacion de nuevos CU:   RU, IS, RS,

Actualizacion de Matriz de trazabilidad TCUR
</commit_message>
<xml_diff>
--- a/PROYECTOS/Proy_SSEL/Libreria en Produccion/Libreria de Trabajo/Documentacion/4. Analisis y Diseño/SSEL-TCUR.xlsx
+++ b/PROYECTOS/Proy_SSEL/Libreria en Produccion/Libreria de Trabajo/Documentacion/4. Analisis y Diseño/SSEL-TCUR.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pulpin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pulpin\Documents\GitHub\FISIDEVELOPS-G3\PROYECTOS\Proy_SSEL\Libreria en Produccion\Libreria de Trabajo\Documentacion\4. Analisis y Diseño\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,22 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
-  <si>
-    <t>CU – 01 Apostar</t>
-  </si>
-  <si>
-    <t>CU – 02 Autenticar</t>
-  </si>
-  <si>
-    <t>CU – 03 Registrar en el sistema</t>
-  </si>
-  <si>
-    <t>CU – 04 Subastar Producto</t>
-  </si>
-  <si>
-    <t>CU – 05 Visualizar subasta</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>MATRIZ DE TRAZABILIDAD CU – REQUISITOS</t>
   </si>
@@ -50,9 +35,6 @@
     <t>RF-06</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>RF-01</t>
   </si>
   <si>
@@ -69,6 +51,54 @@
   </si>
   <si>
     <t>RF-08</t>
+  </si>
+  <si>
+    <t>CU – 01 Registrar Usuario</t>
+  </si>
+  <si>
+    <t>CU – 02 RegistrarSubasta</t>
+  </si>
+  <si>
+    <t>CU – 03 Ingresar al Sistema</t>
+  </si>
+  <si>
+    <t>CU – 04 Recargar Saldo</t>
+  </si>
+  <si>
+    <t>CU – 06  Visualizar Pujas  Realizadas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CU – 05 Visualizar Subasta </t>
+  </si>
+  <si>
+    <t>CU – 07 Visualizar Subasta Realizadas</t>
+  </si>
+  <si>
+    <t>CU – 08 Pujar una Subasta</t>
+  </si>
+  <si>
+    <t>CU – 09 Alta de Usuario</t>
+  </si>
+  <si>
+    <t>CU – 13 Baja de Subasta</t>
+  </si>
+  <si>
+    <t>CU – 10 Baja de Usuario</t>
+  </si>
+  <si>
+    <t>CU – 12 Restablecer Contraseña</t>
+  </si>
+  <si>
+    <t>CU – 11 Visualizar Cuentas</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>RF-09</t>
+  </si>
+  <si>
+    <t>RF-10</t>
   </si>
 </sst>
 </file>
@@ -541,22 +571,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I19"/>
+  <dimension ref="A2:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="11" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:11" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -566,161 +596,264 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="D8" s="3"/>
       <c r="E8" s="4" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-    </row>
-    <row r="13" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="1:11" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -729,18 +862,9 @@
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A3:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>